<commit_message>
Ben fix input with multile file and ouput file zip
</commit_message>
<xml_diff>
--- a/app_demo/output/M0007_0123_5_pos_3_01_287_output.xlsx
+++ b/app_demo/output/M0007_0123_5_pos_3_01_287_output.xlsx
@@ -479,7 +479,7 @@
         <v>81511.0859375</v>
       </c>
       <c r="E2" t="n">
-        <v>5.212476592005957</v>
+        <v>5.21247659109051</v>
       </c>
     </row>
     <row r="3">
@@ -500,7 +500,7 @@
         <v>11200101</v>
       </c>
       <c r="E3" t="n">
-        <v>716.2248376296515</v>
+        <v>716.2248375038637</v>
       </c>
     </row>
     <row r="4">
@@ -521,7 +521,7 @@
         <v>5252337.5</v>
       </c>
       <c r="E4" t="n">
-        <v>4356.548995258208</v>
+        <v>4356.548997543381</v>
       </c>
     </row>
     <row r="5">
@@ -542,7 +542,7 @@
         <v>108706.421875</v>
       </c>
       <c r="E5" t="n">
-        <v>6.951565825765523</v>
+        <v>6.951565824544648</v>
       </c>
     </row>
     <row r="6">
@@ -563,7 +563,7 @@
         <v>99265.71875</v>
       </c>
       <c r="E6" t="n">
-        <v>6.347851085799084</v>
+        <v>6.347851084684235</v>
       </c>
     </row>
     <row r="7">
@@ -584,7 +584,7 @@
         <v>59718.3046875</v>
       </c>
       <c r="E7" t="n">
-        <v>49.53332117078381</v>
+        <v>49.53332119676588</v>
       </c>
     </row>
     <row r="8">
@@ -605,7 +605,7 @@
         <v>364804.1875</v>
       </c>
       <c r="E8" t="n">
-        <v>136.2929689478829</v>
+        <v>136.2929689729838</v>
       </c>
     </row>
     <row r="9">
@@ -626,7 +626,7 @@
         <v>87655.8046875</v>
       </c>
       <c r="E9" t="n">
-        <v>32.74871910941299</v>
+        <v>32.74871911544427</v>
       </c>
     </row>
     <row r="10">
@@ -647,7 +647,7 @@
         <v>180019.25</v>
       </c>
       <c r="E10" t="n">
-        <v>149.3168865699579</v>
+        <v>149.3168866482802</v>
       </c>
     </row>
     <row r="11">
@@ -668,7 +668,7 @@
         <v>205997.796875</v>
       </c>
       <c r="E11" t="n">
-        <v>76.96197657494453</v>
+        <v>76.96197658911851</v>
       </c>
     </row>
     <row r="12">
@@ -689,7 +689,7 @@
         <v>113691.515625</v>
       </c>
       <c r="E12" t="n">
-        <v>7.270352947565795</v>
+        <v>7.270352946288932</v>
       </c>
     </row>
     <row r="13">
@@ -710,7 +710,7 @@
         <v>1606505</v>
       </c>
       <c r="E13" t="n">
-        <v>102.7328934601771</v>
+        <v>102.7328934421345</v>
       </c>
     </row>
     <row r="14">
@@ -731,7 +731,7 @@
         <v>95093.5859375</v>
       </c>
       <c r="E14" t="n">
-        <v>35.52751749956962</v>
+        <v>35.52751750611267</v>
       </c>
     </row>
     <row r="15">
@@ -752,7 +752,7 @@
         <v>545561</v>
       </c>
       <c r="E15" t="n">
-        <v>452.5153279662748</v>
+        <v>452.5153282036359</v>
       </c>
     </row>
     <row r="16">
@@ -773,7 +773,7 @@
         <v>145474.03125</v>
       </c>
       <c r="E16" t="n">
-        <v>54.34994526722532</v>
+        <v>54.34994527723487</v>
       </c>
     </row>
   </sheetData>
@@ -845,7 +845,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>5.212476592005957</t>
+          <t>5.21247659109051</t>
         </is>
       </c>
     </row>
@@ -864,7 +864,7 @@
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Best Match: C(C(F)(F)F)(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F with Similarity: 0.04580152671755725</t>
+          <t>Best Match: C(C(F)(F)F)(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F with Similarity: 0.0458015267175573</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -901,7 +901,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>716.2248376296515</t>
+          <t>716.2248375038637</t>
         </is>
       </c>
     </row>
@@ -920,7 +920,7 @@
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Best Match: C(C(F)(F)F)(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F with Similarity: 0.05128205128205128</t>
+          <t>Best Match: C(C(F)(F)F)(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F with Similarity: 0.0512820512820513</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -957,7 +957,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>4356.548995258208</t>
+          <t>4356.548997543381</t>
         </is>
       </c>
     </row>
@@ -976,7 +976,7 @@
       <c r="A12" t="inlineStr"/>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Best Match: C(C(C(C(F)(F)Cl)(F)F)(F)F)(C(C(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(F)F)(F)F with Similarity: 0.058823529411764705</t>
+          <t>Best Match: C(C(C(C(F)(F)Cl)(F)F)(F)F)(C(C(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(F)F)(F)F with Similarity: 0.0588235294117647</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -1013,7 +1013,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>6.951565825765523</t>
+          <t>6.951565824544648</t>
         </is>
       </c>
     </row>
@@ -1032,7 +1032,7 @@
       <c r="A16" t="inlineStr"/>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Best Match: C(C(F)(F)F)(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F with Similarity: 0.028169014084507043</t>
+          <t>Best Match: C(C(F)(F)F)(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F with Similarity: 0.028169014084507</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
@@ -1069,7 +1069,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>6.347851085799084</t>
+          <t>6.347851084684235</t>
         </is>
       </c>
     </row>
@@ -1088,7 +1088,7 @@
       <c r="A20" t="inlineStr"/>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Best Match: C(C(F)(F)F)(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F with Similarity: 0.022222222222222223</t>
+          <t>Best Match: C(C(F)(F)F)(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F with Similarity: 0.0222222222222222</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>49.53332117078381</t>
+          <t>49.53332119676588</t>
         </is>
       </c>
     </row>
@@ -1144,7 +1144,7 @@
       <c r="A24" t="inlineStr"/>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Best Match: C(C(C(C(F)(F)Cl)(F)F)(F)F)(C(C(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(F)F)(F)F with Similarity: 0.04827586206896552</t>
+          <t>Best Match: C(C(C(C(F)(F)Cl)(F)F)(F)F)(C(C(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(F)F)(F)F with Similarity: 0.0482758620689655</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>136.29296894788294</t>
+          <t>136.29296897298383</t>
         </is>
       </c>
     </row>
@@ -1200,7 +1200,7 @@
       <c r="A28" t="inlineStr"/>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Best Match: C(C(C(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(C(C(F)(F)F)(F)F)(F)F with Similarity: 0.018867924528301886</t>
+          <t>Best Match: C(C(C(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(C(C(F)(F)F)(F)F)(F)F with Similarity: 0.0188679245283019</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>32.74871910941299</t>
+          <t>32.748719115444274</t>
         </is>
       </c>
     </row>
@@ -1256,7 +1256,7 @@
       <c r="A32" t="inlineStr"/>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Best Match: C(C(C(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(C(C(F)(F)F)(F)F)(F)F with Similarity: 0.012048192771084338</t>
+          <t>Best Match: C(C(C(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(C(C(F)(F)F)(F)F)(F)F with Similarity: 0.0120481927710843</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>149.31688656995792</t>
+          <t>149.3168866482802</t>
         </is>
       </c>
     </row>
@@ -1312,7 +1312,7 @@
       <c r="A36" t="inlineStr"/>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Best Match: C(C(C(C(F)(F)Cl)(F)F)(F)F)(C(C(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(F)F)(F)F with Similarity: 0.05063291139240506</t>
+          <t>Best Match: C(C(C(C(F)(F)Cl)(F)F)(F)F)(C(C(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(F)F)(F)F with Similarity: 0.0506329113924051</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>76.96197657494453</t>
+          <t>76.9619765891185</t>
         </is>
       </c>
     </row>
@@ -1368,7 +1368,7 @@
       <c r="A40" t="inlineStr"/>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Best Match: C(C(C(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(C(C(F)(F)F)(F)F)(F)F with Similarity: 0.03571428571428571</t>
+          <t>Best Match: C(C(C(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(C(C(F)(F)F)(F)F)(F)F with Similarity: 0.0357142857142857</t>
         </is>
       </c>
       <c r="C40" t="inlineStr"/>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>7.270352947565795</t>
+          <t>7.270352946288932</t>
         </is>
       </c>
     </row>
@@ -1424,7 +1424,7 @@
       <c r="A44" t="inlineStr"/>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Best Match: C(C(F)(F)F)(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F with Similarity: 0.04285714285714286</t>
+          <t>Best Match: C(C(F)(F)F)(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F with Similarity: 0.0428571428571429</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
@@ -1461,7 +1461,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>102.73289346017712</t>
+          <t>102.73289344213454</t>
         </is>
       </c>
     </row>
@@ -1480,7 +1480,7 @@
       <c r="A48" t="inlineStr"/>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Best Match: C(C(F)(F)F)(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F with Similarity: 0.08974358974358974</t>
+          <t>Best Match: C(C(F)(F)F)(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F with Similarity: 0.0897435897435897</t>
         </is>
       </c>
       <c r="C48" t="inlineStr"/>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>35.52751749956962</t>
+          <t>35.527517506112666</t>
         </is>
       </c>
     </row>
@@ -1536,7 +1536,7 @@
       <c r="A52" t="inlineStr"/>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Best Match: C(C(C(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(C(C(F)(F)F)(F)F)(F)F with Similarity: 0.03296703296703297</t>
+          <t>Best Match: C(C(C(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(C(C(F)(F)F)(F)F)(F)F with Similarity: 0.032967032967033</t>
         </is>
       </c>
       <c r="C52" t="inlineStr"/>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>452.51532796627475</t>
+          <t>452.5153282036359</t>
         </is>
       </c>
     </row>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>54.34994526722532</t>
+          <t>54.349945277234866</t>
         </is>
       </c>
     </row>
@@ -1648,7 +1648,7 @@
       <c r="A60" t="inlineStr"/>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Best Match: C(C(C(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(C(C(F)(F)F)(F)F)(F)F with Similarity: 0.03333333333333333</t>
+          <t>Best Match: C(C(C(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(C(C(F)(F)F)(F)F)(F)F with Similarity: 0.0333333333333333</t>
         </is>
       </c>
       <c r="C60" t="inlineStr"/>

</xml_diff>